<commit_message>
some changes regading to data format in cluster master upload template file
</commit_message>
<xml_diff>
--- a/src/assets/Download/ClusterMasterTemplate.xlsx
+++ b/src/assets/Download/ClusterMasterTemplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>ClusterName</t>
   </si>
@@ -41,16 +41,28 @@
     <t>Mayapuri</t>
   </si>
   <si>
+    <t>110030</t>
+  </si>
+  <si>
     <t>Area</t>
   </si>
   <si>
     <t>Mandoli</t>
   </si>
   <si>
+    <t>110057</t>
+  </si>
+  <si>
     <t>Wazirpur</t>
   </si>
   <si>
+    <t>110045</t>
+  </si>
+  <si>
     <t>Mahipalpur</t>
+  </si>
+  <si>
+    <t>110037</t>
   </si>
 </sst>
 </file>
@@ -63,7 +75,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +97,6 @@
       <name val="Calibri Light"/>
       <charset val="134"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -562,155 +567,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,70 +1041,70 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="14.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="9.42857142857143" customWidth="1"/>
+    <col min="2" max="2" width="9.42857142857143" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="7.28571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>110030</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>110057</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
-        <v>110045</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>110037</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>